<commit_message>
Adding the aggregation mock to the tests
- Adding a dummy mock for IOT_aggrgation
</commit_message>
<xml_diff>
--- a/mario/test/IOT.xlsx
+++ b/mario/test/IOT.xlsx
@@ -1,22 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10215"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\payam\Documents\GitHub\MARIO\mario\test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mohammadamintahavori/Documents/GitHub/MARIO/mario/test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F36E0A6-BFF2-4B56-9E3E-3DDF0B87C78C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA3E0618-F780-EB44-A2CE-78A3AFD4DB2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4128" yWindow="444" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4120" yWindow="500" windowWidth="17280" windowHeight="8960" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="flows" sheetId="1" r:id="rId1"/>
     <sheet name="units" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -128,7 +140,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -138,6 +150,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -169,12 +187,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -515,29 +534,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView topLeftCell="E1" zoomScale="109" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="P1" sqref="P1:Q3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.5" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.5" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="14" max="15" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="22.5546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="22.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
@@ -581,7 +600,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="D2" s="1" t="s">
         <v>1</v>
       </c>
@@ -625,7 +644,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="D3" s="1" t="s">
         <v>2</v>
       </c>
@@ -669,7 +688,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -679,40 +698,40 @@
       <c r="C4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="3">
         <v>679633.57952100004</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="3">
         <v>12742.739781677999</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="3">
         <v>2856303.7693596738</v>
       </c>
-      <c r="G4" s="2">
+      <c r="G4" s="3">
         <v>483389.77788244269</v>
       </c>
-      <c r="H4" s="2">
+      <c r="H4" s="3">
         <v>81223.536805420503</v>
       </c>
-      <c r="I4" s="2">
+      <c r="I4" s="3">
         <v>74896.983985559549</v>
       </c>
-      <c r="J4" s="2">
+      <c r="J4" s="3">
         <v>1937.994943097724</v>
       </c>
-      <c r="K4" s="2">
+      <c r="K4" s="3">
         <v>3.7691765935912702</v>
       </c>
-      <c r="L4" s="2">
+      <c r="L4" s="3">
         <v>5765.2557998694519</v>
       </c>
-      <c r="M4" s="2">
+      <c r="M4" s="3">
         <v>1398.158814124334</v>
       </c>
-      <c r="N4" s="2">
+      <c r="N4" s="3">
         <v>228.33025329716389</v>
       </c>
-      <c r="O4" s="2">
+      <c r="O4" s="3">
         <v>42.026541375617519</v>
       </c>
       <c r="P4" s="2">
@@ -722,7 +741,7 @@
         <v>10993.172377756189</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -732,40 +751,40 @@
       <c r="C5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="3">
         <v>13838.769405880879</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="3">
         <v>224649.99660834731</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5" s="3">
         <v>2501495.2277574451</v>
       </c>
-      <c r="G5" s="2">
+      <c r="G5" s="3">
         <v>270843.05301922659</v>
       </c>
-      <c r="H5" s="2">
+      <c r="H5" s="3">
         <v>142131.14312528499</v>
       </c>
-      <c r="I5" s="2">
+      <c r="I5" s="3">
         <v>22793.81387289289</v>
       </c>
-      <c r="J5" s="2">
+      <c r="J5" s="3">
         <v>41.807221560881707</v>
       </c>
-      <c r="K5" s="2">
+      <c r="K5" s="3">
         <v>379.45820693116798</v>
       </c>
-      <c r="L5" s="2">
+      <c r="L5" s="3">
         <v>44842.551061536222</v>
       </c>
-      <c r="M5" s="2">
+      <c r="M5" s="3">
         <v>8331.4238853705247</v>
       </c>
-      <c r="N5" s="2">
+      <c r="N5" s="3">
         <v>128.31224417861699</v>
       </c>
-      <c r="O5" s="2">
+      <c r="O5" s="3">
         <v>213.66437179296159</v>
       </c>
       <c r="P5" s="2">
@@ -775,7 +794,7 @@
         <v>462.17243687258963</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>0</v>
       </c>
@@ -785,40 +804,40 @@
       <c r="C6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="3">
         <v>747904.55887745356</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="3">
         <v>374491.94826940238</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F6" s="3">
         <v>22892840.599005181</v>
       </c>
-      <c r="G6" s="2">
+      <c r="G6" s="3">
         <v>5710993.0160787823</v>
       </c>
-      <c r="H6" s="2">
+      <c r="H6" s="3">
         <v>3964746.712965542</v>
       </c>
-      <c r="I6" s="2">
+      <c r="I6" s="3">
         <v>975215.46352448617</v>
       </c>
-      <c r="J6" s="2">
+      <c r="J6" s="3">
         <v>1226.982579162624</v>
       </c>
-      <c r="K6" s="2">
+      <c r="K6" s="3">
         <v>186.7146398688634</v>
       </c>
-      <c r="L6" s="2">
+      <c r="L6" s="3">
         <v>134910.65754329169</v>
       </c>
-      <c r="M6" s="2">
+      <c r="M6" s="3">
         <v>22456.821703749611</v>
       </c>
-      <c r="N6" s="2">
+      <c r="N6" s="3">
         <v>5354.3400048172298</v>
       </c>
-      <c r="O6" s="2">
+      <c r="O6" s="3">
         <v>2556.0480006031239</v>
       </c>
       <c r="P6" s="2">
@@ -828,7 +847,7 @@
         <v>121750.6625725599</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>0</v>
       </c>
@@ -838,40 +857,40 @@
       <c r="C7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="3">
         <v>983380.50950405747</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" s="3">
         <v>577951.4000950132</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F7" s="3">
         <v>8223528.4636955792</v>
       </c>
-      <c r="G7" s="2">
+      <c r="G7" s="3">
         <v>21539516.783423498</v>
       </c>
-      <c r="H7" s="2">
+      <c r="H7" s="3">
         <v>1921259.1831035551</v>
       </c>
-      <c r="I7" s="2">
+      <c r="I7" s="3">
         <v>1405010.1735635479</v>
       </c>
-      <c r="J7" s="2">
+      <c r="J7" s="3">
         <v>770.49133115541451</v>
       </c>
-      <c r="K7" s="2">
+      <c r="K7" s="3">
         <v>312.75387304949328</v>
       </c>
-      <c r="L7" s="2">
+      <c r="L7" s="3">
         <v>22834.324684092931</v>
       </c>
-      <c r="M7" s="2">
+      <c r="M7" s="3">
         <v>37496.066601641112</v>
       </c>
-      <c r="N7" s="2">
+      <c r="N7" s="3">
         <v>2289.707911616284</v>
       </c>
-      <c r="O7" s="2">
+      <c r="O7" s="3">
         <v>3453.8610203772159</v>
       </c>
       <c r="P7" s="2">
@@ -881,7 +900,7 @@
         <v>43071.682787637117</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>0</v>
       </c>
@@ -891,40 +910,40 @@
       <c r="C8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8" s="3">
         <v>22837.66098632853</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8" s="3">
         <v>45939.595199216223</v>
       </c>
-      <c r="F8" s="2">
+      <c r="F8" s="3">
         <v>152873.14002278959</v>
       </c>
-      <c r="G8" s="2">
+      <c r="G8" s="3">
         <v>938957.67146317218</v>
       </c>
-      <c r="H8" s="2">
+      <c r="H8" s="3">
         <v>866542.69216097472</v>
       </c>
-      <c r="I8" s="2">
+      <c r="I8" s="3">
         <v>42035.809478375457</v>
       </c>
-      <c r="J8" s="2">
+      <c r="J8" s="3">
         <v>7.304333537659236</v>
       </c>
-      <c r="K8" s="2">
+      <c r="K8" s="3">
         <v>3.4882123571827059</v>
       </c>
-      <c r="L8" s="2">
+      <c r="L8" s="3">
         <v>390.20442035944092</v>
       </c>
-      <c r="M8" s="2">
+      <c r="M8" s="3">
         <v>197.8382652784405</v>
       </c>
-      <c r="N8" s="2">
+      <c r="N8" s="3">
         <v>731.10576011293961</v>
       </c>
-      <c r="O8" s="2">
+      <c r="O8" s="3">
         <v>15.01225071768226</v>
       </c>
       <c r="P8" s="2">
@@ -934,7 +953,7 @@
         <v>1072.0442986401911</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>0</v>
       </c>
@@ -944,40 +963,40 @@
       <c r="C9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9" s="3">
         <v>126874.6668469915</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E9" s="3">
         <v>136601.9521290363</v>
       </c>
-      <c r="F9" s="2">
+      <c r="F9" s="3">
         <v>1361107.2097869739</v>
       </c>
-      <c r="G9" s="2">
+      <c r="G9" s="3">
         <v>1925954.3083199931</v>
       </c>
-      <c r="H9" s="2">
+      <c r="H9" s="3">
         <v>543692.18828156032</v>
       </c>
-      <c r="I9" s="2">
+      <c r="I9" s="3">
         <v>1414883.4169662951</v>
       </c>
-      <c r="J9" s="2">
+      <c r="J9" s="3">
         <v>90.501725455622861</v>
       </c>
-      <c r="K9" s="2">
+      <c r="K9" s="3">
         <v>117.1857248838752</v>
       </c>
-      <c r="L9" s="2">
+      <c r="L9" s="3">
         <v>4589.3281116194576</v>
       </c>
-      <c r="M9" s="2">
+      <c r="M9" s="3">
         <v>7549.7200751604087</v>
       </c>
-      <c r="N9" s="2">
+      <c r="N9" s="3">
         <v>140.57236827806429</v>
       </c>
-      <c r="O9" s="2">
+      <c r="O9" s="3">
         <v>6651.5000011331822</v>
       </c>
       <c r="P9" s="2">
@@ -987,7 +1006,7 @@
         <v>8726.0206972874184</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -997,40 +1016,40 @@
       <c r="C10" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10" s="3">
         <v>317.11677117300729</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E10" s="3">
         <v>5.121087662275726</v>
       </c>
-      <c r="F10" s="2">
+      <c r="F10" s="3">
         <v>1294.2306995571971</v>
       </c>
-      <c r="G10" s="2">
+      <c r="G10" s="3">
         <v>379.83021836899809</v>
       </c>
-      <c r="H10" s="2">
+      <c r="H10" s="3">
         <v>22.472907804328539</v>
       </c>
-      <c r="I10" s="2">
+      <c r="I10" s="3">
         <v>16.898415427875701</v>
       </c>
-      <c r="J10" s="2">
+      <c r="J10" s="3">
         <v>2326.0444769715809</v>
       </c>
-      <c r="K10" s="2">
+      <c r="K10" s="3">
         <v>1.1302794905942311</v>
       </c>
-      <c r="L10" s="2">
+      <c r="L10" s="3">
         <v>25126.335538085801</v>
       </c>
-      <c r="M10" s="2">
+      <c r="M10" s="3">
         <v>3241.0823027316228</v>
       </c>
-      <c r="N10" s="2">
+      <c r="N10" s="3">
         <v>137.70535231925311</v>
       </c>
-      <c r="O10" s="2">
+      <c r="O10" s="3">
         <v>78.883464140914384</v>
       </c>
       <c r="P10" s="2">
@@ -1040,7 +1059,7 @@
         <v>28434.707841273332</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
@@ -1050,40 +1069,40 @@
       <c r="C11" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11" s="3">
         <v>17.9251641316168</v>
       </c>
-      <c r="E11" s="2">
+      <c r="E11" s="3">
         <v>76.695695812088076</v>
       </c>
-      <c r="F11" s="2">
+      <c r="F11" s="3">
         <v>1301.8101954977139</v>
       </c>
-      <c r="G11" s="2">
+      <c r="G11" s="3">
         <v>173.52428449068731</v>
       </c>
-      <c r="H11" s="2">
+      <c r="H11" s="3">
         <v>241.02294827930689</v>
       </c>
-      <c r="I11" s="2">
+      <c r="I11" s="3">
         <v>9.2583317458404437</v>
       </c>
-      <c r="J11" s="2">
+      <c r="J11" s="3">
         <v>38.421370980919917</v>
       </c>
-      <c r="K11" s="2">
+      <c r="K11" s="3">
         <v>596.96161035144348</v>
       </c>
-      <c r="L11" s="2">
+      <c r="L11" s="3">
         <v>5508.7101578150896</v>
       </c>
-      <c r="M11" s="2">
+      <c r="M11" s="3">
         <v>2762.4863736441312</v>
       </c>
-      <c r="N11" s="2">
+      <c r="N11" s="3">
         <v>1647.5535350682669</v>
       </c>
-      <c r="O11" s="2">
+      <c r="O11" s="3">
         <v>93.932871865263479</v>
       </c>
       <c r="P11" s="2">
@@ -1093,7 +1112,7 @@
         <v>921.99215744640492</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>8</v>
       </c>
@@ -1103,40 +1122,40 @@
       <c r="C12" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D12" s="2">
+      <c r="D12" s="3">
         <v>3649.1993663425301</v>
       </c>
-      <c r="E12" s="2">
+      <c r="E12" s="3">
         <v>3241.787337001017</v>
       </c>
-      <c r="F12" s="2">
+      <c r="F12" s="3">
         <v>133519.32066834779</v>
       </c>
-      <c r="G12" s="2">
+      <c r="G12" s="3">
         <v>34544.694231030917</v>
       </c>
-      <c r="H12" s="2">
+      <c r="H12" s="3">
         <v>24209.885076749739</v>
       </c>
-      <c r="I12" s="2">
+      <c r="I12" s="3">
         <v>6803.7122235240222</v>
       </c>
-      <c r="J12" s="2">
+      <c r="J12" s="3">
         <v>8757.4835845585276</v>
       </c>
-      <c r="K12" s="2">
+      <c r="K12" s="3">
         <v>979.44838741463775</v>
       </c>
-      <c r="L12" s="2">
+      <c r="L12" s="3">
         <v>287300.67335464072</v>
       </c>
-      <c r="M12" s="2">
+      <c r="M12" s="3">
         <v>95627.544506457925</v>
       </c>
-      <c r="N12" s="2">
+      <c r="N12" s="3">
         <v>50163.11487806381</v>
       </c>
-      <c r="O12" s="2">
+      <c r="O12" s="3">
         <v>15336.28122936241</v>
       </c>
       <c r="P12" s="2">
@@ -1146,7 +1165,7 @@
         <v>299898.91113128111</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>8</v>
       </c>
@@ -1199,7 +1218,7 @@
         <v>1052846.501297662</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>8</v>
       </c>
@@ -1252,7 +1271,7 @@
         <v>144773.15982211279</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>8</v>
       </c>
@@ -1305,7 +1324,7 @@
         <v>57385.248142014359</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>9</v>
       </c>
@@ -1358,7 +1377,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>9</v>
       </c>
@@ -1411,7 +1430,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>9</v>
       </c>
@@ -1464,7 +1483,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>9</v>
       </c>
@@ -1517,7 +1536,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>9</v>
       </c>
@@ -1540,7 +1559,7 @@
         <v>15947800328396.711</v>
       </c>
       <c r="H20" s="2">
-        <v>341641828013.82813</v>
+        <v>341641828013.82812</v>
       </c>
       <c r="I20" s="2">
         <v>2497930396711.436</v>
@@ -1570,7 +1589,7 @@
         <v>69021047159.929993</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>9</v>
       </c>
@@ -1623,7 +1642,7 @@
         <v>381.09674629800003</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>9</v>
       </c>
@@ -1685,23 +1704,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C1" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>14</v>
       </c>
@@ -1712,7 +1731,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>14</v>
       </c>
@@ -1723,7 +1742,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>14</v>
       </c>
@@ -1734,7 +1753,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>14</v>
       </c>
@@ -1745,7 +1764,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
@@ -1756,7 +1775,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
@@ -1767,7 +1786,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
@@ -1778,7 +1797,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>1</v>
       </c>
@@ -1789,7 +1808,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>1</v>
       </c>
@@ -1800,7 +1819,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>1</v>
       </c>
@@ -1811,7 +1830,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>1</v>
       </c>
@@ -1822,7 +1841,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>1</v>
       </c>
@@ -1833,7 +1852,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
Revert "Merge pull request #29 from SESAM-Polimi/unit_test"
This reverts commit cdf8994089466c8647a733f3f8c9ec509fc194be, reversing
changes made to 49ee514b5b26fa43cf572a4dbf8ce9e0ef11f4c3.
</commit_message>
<xml_diff>
--- a/mario/test/IOT.xlsx
+++ b/mario/test/IOT.xlsx
@@ -1,34 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10215"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mohammadamintahavori/Documents/GitHub/MARIO/mario/test/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\payam\Documents\GitHub\MARIO\mario\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA3E0618-F780-EB44-A2CE-78A3AFD4DB2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F36E0A6-BFF2-4B56-9E3E-3DDF0B87C78C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4120" yWindow="500" windowWidth="17280" windowHeight="8960" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4128" yWindow="444" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="flows" sheetId="1" r:id="rId1"/>
     <sheet name="units" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -140,7 +128,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -150,12 +138,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -187,13 +169,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -534,29 +515,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q22"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScale="109" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="P1" sqref="P1:Q3"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.5546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.44140625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="14" max="15" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="22.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
@@ -600,7 +581,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="D2" s="1" t="s">
         <v>1</v>
       </c>
@@ -644,7 +625,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="D3" s="1" t="s">
         <v>2</v>
       </c>
@@ -688,7 +669,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -698,40 +679,40 @@
       <c r="C4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="2">
         <v>679633.57952100004</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="2">
         <v>12742.739781677999</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="2">
         <v>2856303.7693596738</v>
       </c>
-      <c r="G4" s="3">
+      <c r="G4" s="2">
         <v>483389.77788244269</v>
       </c>
-      <c r="H4" s="3">
+      <c r="H4" s="2">
         <v>81223.536805420503</v>
       </c>
-      <c r="I4" s="3">
+      <c r="I4" s="2">
         <v>74896.983985559549</v>
       </c>
-      <c r="J4" s="3">
+      <c r="J4" s="2">
         <v>1937.994943097724</v>
       </c>
-      <c r="K4" s="3">
+      <c r="K4" s="2">
         <v>3.7691765935912702</v>
       </c>
-      <c r="L4" s="3">
+      <c r="L4" s="2">
         <v>5765.2557998694519</v>
       </c>
-      <c r="M4" s="3">
+      <c r="M4" s="2">
         <v>1398.158814124334</v>
       </c>
-      <c r="N4" s="3">
+      <c r="N4" s="2">
         <v>228.33025329716389</v>
       </c>
-      <c r="O4" s="3">
+      <c r="O4" s="2">
         <v>42.026541375617519</v>
       </c>
       <c r="P4" s="2">
@@ -741,7 +722,7 @@
         <v>10993.172377756189</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -751,40 +732,40 @@
       <c r="C5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="2">
         <v>13838.769405880879</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="2">
         <v>224649.99660834731</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5" s="2">
         <v>2501495.2277574451</v>
       </c>
-      <c r="G5" s="3">
+      <c r="G5" s="2">
         <v>270843.05301922659</v>
       </c>
-      <c r="H5" s="3">
+      <c r="H5" s="2">
         <v>142131.14312528499</v>
       </c>
-      <c r="I5" s="3">
+      <c r="I5" s="2">
         <v>22793.81387289289</v>
       </c>
-      <c r="J5" s="3">
+      <c r="J5" s="2">
         <v>41.807221560881707</v>
       </c>
-      <c r="K5" s="3">
+      <c r="K5" s="2">
         <v>379.45820693116798</v>
       </c>
-      <c r="L5" s="3">
+      <c r="L5" s="2">
         <v>44842.551061536222</v>
       </c>
-      <c r="M5" s="3">
+      <c r="M5" s="2">
         <v>8331.4238853705247</v>
       </c>
-      <c r="N5" s="3">
+      <c r="N5" s="2">
         <v>128.31224417861699</v>
       </c>
-      <c r="O5" s="3">
+      <c r="O5" s="2">
         <v>213.66437179296159</v>
       </c>
       <c r="P5" s="2">
@@ -794,7 +775,7 @@
         <v>462.17243687258963</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>0</v>
       </c>
@@ -804,40 +785,40 @@
       <c r="C6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="2">
         <v>747904.55887745356</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="2">
         <v>374491.94826940238</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="2">
         <v>22892840.599005181</v>
       </c>
-      <c r="G6" s="3">
+      <c r="G6" s="2">
         <v>5710993.0160787823</v>
       </c>
-      <c r="H6" s="3">
+      <c r="H6" s="2">
         <v>3964746.712965542</v>
       </c>
-      <c r="I6" s="3">
+      <c r="I6" s="2">
         <v>975215.46352448617</v>
       </c>
-      <c r="J6" s="3">
+      <c r="J6" s="2">
         <v>1226.982579162624</v>
       </c>
-      <c r="K6" s="3">
+      <c r="K6" s="2">
         <v>186.7146398688634</v>
       </c>
-      <c r="L6" s="3">
+      <c r="L6" s="2">
         <v>134910.65754329169</v>
       </c>
-      <c r="M6" s="3">
+      <c r="M6" s="2">
         <v>22456.821703749611</v>
       </c>
-      <c r="N6" s="3">
+      <c r="N6" s="2">
         <v>5354.3400048172298</v>
       </c>
-      <c r="O6" s="3">
+      <c r="O6" s="2">
         <v>2556.0480006031239</v>
       </c>
       <c r="P6" s="2">
@@ -847,7 +828,7 @@
         <v>121750.6625725599</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>0</v>
       </c>
@@ -857,40 +838,40 @@
       <c r="C7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="2">
         <v>983380.50950405747</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="2">
         <v>577951.4000950132</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7" s="2">
         <v>8223528.4636955792</v>
       </c>
-      <c r="G7" s="3">
+      <c r="G7" s="2">
         <v>21539516.783423498</v>
       </c>
-      <c r="H7" s="3">
+      <c r="H7" s="2">
         <v>1921259.1831035551</v>
       </c>
-      <c r="I7" s="3">
+      <c r="I7" s="2">
         <v>1405010.1735635479</v>
       </c>
-      <c r="J7" s="3">
+      <c r="J7" s="2">
         <v>770.49133115541451</v>
       </c>
-      <c r="K7" s="3">
+      <c r="K7" s="2">
         <v>312.75387304949328</v>
       </c>
-      <c r="L7" s="3">
+      <c r="L7" s="2">
         <v>22834.324684092931</v>
       </c>
-      <c r="M7" s="3">
+      <c r="M7" s="2">
         <v>37496.066601641112</v>
       </c>
-      <c r="N7" s="3">
+      <c r="N7" s="2">
         <v>2289.707911616284</v>
       </c>
-      <c r="O7" s="3">
+      <c r="O7" s="2">
         <v>3453.8610203772159</v>
       </c>
       <c r="P7" s="2">
@@ -900,7 +881,7 @@
         <v>43071.682787637117</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>0</v>
       </c>
@@ -910,40 +891,40 @@
       <c r="C8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="2">
         <v>22837.66098632853</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="2">
         <v>45939.595199216223</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F8" s="2">
         <v>152873.14002278959</v>
       </c>
-      <c r="G8" s="3">
+      <c r="G8" s="2">
         <v>938957.67146317218</v>
       </c>
-      <c r="H8" s="3">
+      <c r="H8" s="2">
         <v>866542.69216097472</v>
       </c>
-      <c r="I8" s="3">
+      <c r="I8" s="2">
         <v>42035.809478375457</v>
       </c>
-      <c r="J8" s="3">
+      <c r="J8" s="2">
         <v>7.304333537659236</v>
       </c>
-      <c r="K8" s="3">
+      <c r="K8" s="2">
         <v>3.4882123571827059</v>
       </c>
-      <c r="L8" s="3">
+      <c r="L8" s="2">
         <v>390.20442035944092</v>
       </c>
-      <c r="M8" s="3">
+      <c r="M8" s="2">
         <v>197.8382652784405</v>
       </c>
-      <c r="N8" s="3">
+      <c r="N8" s="2">
         <v>731.10576011293961</v>
       </c>
-      <c r="O8" s="3">
+      <c r="O8" s="2">
         <v>15.01225071768226</v>
       </c>
       <c r="P8" s="2">
@@ -953,7 +934,7 @@
         <v>1072.0442986401911</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>0</v>
       </c>
@@ -963,40 +944,40 @@
       <c r="C9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9" s="2">
         <v>126874.6668469915</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="2">
         <v>136601.9521290363</v>
       </c>
-      <c r="F9" s="3">
+      <c r="F9" s="2">
         <v>1361107.2097869739</v>
       </c>
-      <c r="G9" s="3">
+      <c r="G9" s="2">
         <v>1925954.3083199931</v>
       </c>
-      <c r="H9" s="3">
+      <c r="H9" s="2">
         <v>543692.18828156032</v>
       </c>
-      <c r="I9" s="3">
+      <c r="I9" s="2">
         <v>1414883.4169662951</v>
       </c>
-      <c r="J9" s="3">
+      <c r="J9" s="2">
         <v>90.501725455622861</v>
       </c>
-      <c r="K9" s="3">
+      <c r="K9" s="2">
         <v>117.1857248838752</v>
       </c>
-      <c r="L9" s="3">
+      <c r="L9" s="2">
         <v>4589.3281116194576</v>
       </c>
-      <c r="M9" s="3">
+      <c r="M9" s="2">
         <v>7549.7200751604087</v>
       </c>
-      <c r="N9" s="3">
+      <c r="N9" s="2">
         <v>140.57236827806429</v>
       </c>
-      <c r="O9" s="3">
+      <c r="O9" s="2">
         <v>6651.5000011331822</v>
       </c>
       <c r="P9" s="2">
@@ -1006,7 +987,7 @@
         <v>8726.0206972874184</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -1016,40 +997,40 @@
       <c r="C10" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10" s="2">
         <v>317.11677117300729</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10" s="2">
         <v>5.121087662275726</v>
       </c>
-      <c r="F10" s="3">
+      <c r="F10" s="2">
         <v>1294.2306995571971</v>
       </c>
-      <c r="G10" s="3">
+      <c r="G10" s="2">
         <v>379.83021836899809</v>
       </c>
-      <c r="H10" s="3">
+      <c r="H10" s="2">
         <v>22.472907804328539</v>
       </c>
-      <c r="I10" s="3">
+      <c r="I10" s="2">
         <v>16.898415427875701</v>
       </c>
-      <c r="J10" s="3">
+      <c r="J10" s="2">
         <v>2326.0444769715809</v>
       </c>
-      <c r="K10" s="3">
+      <c r="K10" s="2">
         <v>1.1302794905942311</v>
       </c>
-      <c r="L10" s="3">
+      <c r="L10" s="2">
         <v>25126.335538085801</v>
       </c>
-      <c r="M10" s="3">
+      <c r="M10" s="2">
         <v>3241.0823027316228</v>
       </c>
-      <c r="N10" s="3">
+      <c r="N10" s="2">
         <v>137.70535231925311</v>
       </c>
-      <c r="O10" s="3">
+      <c r="O10" s="2">
         <v>78.883464140914384</v>
       </c>
       <c r="P10" s="2">
@@ -1059,7 +1040,7 @@
         <v>28434.707841273332</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
@@ -1069,40 +1050,40 @@
       <c r="C11" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D11" s="3">
+      <c r="D11" s="2">
         <v>17.9251641316168</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E11" s="2">
         <v>76.695695812088076</v>
       </c>
-      <c r="F11" s="3">
+      <c r="F11" s="2">
         <v>1301.8101954977139</v>
       </c>
-      <c r="G11" s="3">
+      <c r="G11" s="2">
         <v>173.52428449068731</v>
       </c>
-      <c r="H11" s="3">
+      <c r="H11" s="2">
         <v>241.02294827930689</v>
       </c>
-      <c r="I11" s="3">
+      <c r="I11" s="2">
         <v>9.2583317458404437</v>
       </c>
-      <c r="J11" s="3">
+      <c r="J11" s="2">
         <v>38.421370980919917</v>
       </c>
-      <c r="K11" s="3">
+      <c r="K11" s="2">
         <v>596.96161035144348</v>
       </c>
-      <c r="L11" s="3">
+      <c r="L11" s="2">
         <v>5508.7101578150896</v>
       </c>
-      <c r="M11" s="3">
+      <c r="M11" s="2">
         <v>2762.4863736441312</v>
       </c>
-      <c r="N11" s="3">
+      <c r="N11" s="2">
         <v>1647.5535350682669</v>
       </c>
-      <c r="O11" s="3">
+      <c r="O11" s="2">
         <v>93.932871865263479</v>
       </c>
       <c r="P11" s="2">
@@ -1112,7 +1093,7 @@
         <v>921.99215744640492</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>8</v>
       </c>
@@ -1122,40 +1103,40 @@
       <c r="C12" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D12" s="2">
         <v>3649.1993663425301</v>
       </c>
-      <c r="E12" s="3">
+      <c r="E12" s="2">
         <v>3241.787337001017</v>
       </c>
-      <c r="F12" s="3">
+      <c r="F12" s="2">
         <v>133519.32066834779</v>
       </c>
-      <c r="G12" s="3">
+      <c r="G12" s="2">
         <v>34544.694231030917</v>
       </c>
-      <c r="H12" s="3">
+      <c r="H12" s="2">
         <v>24209.885076749739</v>
       </c>
-      <c r="I12" s="3">
+      <c r="I12" s="2">
         <v>6803.7122235240222</v>
       </c>
-      <c r="J12" s="3">
+      <c r="J12" s="2">
         <v>8757.4835845585276</v>
       </c>
-      <c r="K12" s="3">
+      <c r="K12" s="2">
         <v>979.44838741463775</v>
       </c>
-      <c r="L12" s="3">
+      <c r="L12" s="2">
         <v>287300.67335464072</v>
       </c>
-      <c r="M12" s="3">
+      <c r="M12" s="2">
         <v>95627.544506457925</v>
       </c>
-      <c r="N12" s="3">
+      <c r="N12" s="2">
         <v>50163.11487806381</v>
       </c>
-      <c r="O12" s="3">
+      <c r="O12" s="2">
         <v>15336.28122936241</v>
       </c>
       <c r="P12" s="2">
@@ -1165,7 +1146,7 @@
         <v>299898.91113128111</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>8</v>
       </c>
@@ -1218,7 +1199,7 @@
         <v>1052846.501297662</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>8</v>
       </c>
@@ -1271,7 +1252,7 @@
         <v>144773.15982211279</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>8</v>
       </c>
@@ -1324,7 +1305,7 @@
         <v>57385.248142014359</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>9</v>
       </c>
@@ -1377,7 +1358,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>9</v>
       </c>
@@ -1430,7 +1411,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>9</v>
       </c>
@@ -1483,7 +1464,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>9</v>
       </c>
@@ -1536,7 +1517,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>9</v>
       </c>
@@ -1559,7 +1540,7 @@
         <v>15947800328396.711</v>
       </c>
       <c r="H20" s="2">
-        <v>341641828013.82812</v>
+        <v>341641828013.82813</v>
       </c>
       <c r="I20" s="2">
         <v>2497930396711.436</v>
@@ -1589,7 +1570,7 @@
         <v>69021047159.929993</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>9</v>
       </c>
@@ -1642,7 +1623,7 @@
         <v>381.09674629800003</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>9</v>
       </c>
@@ -1704,23 +1685,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C1" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>14</v>
       </c>
@@ -1731,7 +1712,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>14</v>
       </c>
@@ -1742,7 +1723,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>14</v>
       </c>
@@ -1753,7 +1734,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>14</v>
       </c>
@@ -1764,7 +1745,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
@@ -1775,7 +1756,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
@@ -1786,7 +1767,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
@@ -1797,7 +1778,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>1</v>
       </c>
@@ -1808,7 +1789,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>1</v>
       </c>
@@ -1819,7 +1800,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>1</v>
       </c>
@@ -1830,7 +1811,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>1</v>
       </c>
@@ -1841,7 +1822,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>1</v>
       </c>
@@ -1852,7 +1833,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>1</v>
       </c>

</xml_diff>